<commit_message>
Update expected values for insects, mech rem, add and wind
</commit_message>
<xml_diff>
--- a/specifications/4_Wind/ScriptRules_Wind.xlsx
+++ b/specifications/4_Wind/ScriptRules_Wind.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12465" windowHeight="9930" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12465" windowHeight="9930" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -2720,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K951"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="B34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7428,8 +7428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC951"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView topLeftCell="B63" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7438,10 +7438,10 @@
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="13" width="18.5703125" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
@@ -7672,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="14">
-        <f t="shared" ref="M3:M47" si="3">L3</f>
+        <f t="shared" ref="M3:M66" si="3">L3</f>
         <v>0</v>
       </c>
       <c r="O3" s="10">
@@ -7684,7 +7684,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="14">
-        <f t="shared" ref="Q3:Q47" si="5">P3</f>
+        <f t="shared" ref="Q3:Q66" si="5">P3</f>
         <v>0</v>
       </c>
       <c r="R3" s="9">
@@ -7699,7 +7699,7 @@
         <v>2.9</v>
       </c>
       <c r="U3" s="14">
-        <f t="shared" ref="U3:U47" si="7">T3</f>
+        <f t="shared" ref="U3:U66" si="7">T3</f>
         <v>2.9</v>
       </c>
       <c r="V3" s="9">
@@ -7714,7 +7714,7 @@
         <v>14</v>
       </c>
       <c r="Y3" s="14">
-        <f t="shared" ref="Y3:Y47" si="9">X3</f>
+        <f t="shared" ref="Y3:Y66" si="9">X3</f>
         <v>14</v>
       </c>
       <c r="Z3" s="9">
@@ -7729,7 +7729,7 @@
         <v>12</v>
       </c>
       <c r="AC3" s="14">
-        <f t="shared" ref="AC3:AC47" si="11">AB3</f>
+        <f t="shared" ref="AC3:AC66" si="11">AB3</f>
         <v>12</v>
       </c>
     </row>
@@ -11767,7 +11767,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="13">
-        <f t="shared" ref="L47" si="25">K47</f>
+        <f t="shared" ref="L47:L93" si="25">K47</f>
         <v>0</v>
       </c>
       <c r="M47" s="14">
@@ -11782,7 +11782,7 @@
         <v>70</v>
       </c>
       <c r="P47" s="13">
-        <f t="shared" ref="P47" si="26">O47</f>
+        <f t="shared" ref="P47:P93" si="26">O47</f>
         <v>70</v>
       </c>
       <c r="Q47" s="14">
@@ -11797,7 +11797,7 @@
         <v>90</v>
       </c>
       <c r="T47" s="13">
-        <f t="shared" ref="T47" si="27">S47</f>
+        <f t="shared" ref="T47:T93" si="27">S47</f>
         <v>90</v>
       </c>
       <c r="U47" s="14">
@@ -11809,7 +11809,7 @@
         <v>0</v>
       </c>
       <c r="X47" s="13">
-        <f t="shared" ref="X47" si="28">W47</f>
+        <f t="shared" ref="X47:X93" si="28">W47</f>
         <v>0</v>
       </c>
       <c r="Y47" s="14">
@@ -11824,7 +11824,7 @@
         <v>60</v>
       </c>
       <c r="AB47" s="13">
-        <f t="shared" ref="AB47" si="29">AA47</f>
+        <f t="shared" ref="AB47:AB93" si="29">AA47</f>
         <v>60</v>
       </c>
       <c r="AC47" s="14">
@@ -11852,7 +11852,7 @@
         <v>4</v>
       </c>
       <c r="G48" s="10">
-        <f>MAX(1,$C48*F48)</f>
+        <f>$C48*F48</f>
         <v>5</v>
       </c>
       <c r="H48" s="13">
@@ -11867,7 +11867,7 @@
         <v>1</v>
       </c>
       <c r="K48" s="10">
-        <f>MAX(1,$C48*J48)</f>
+        <f>$C48*J48</f>
         <v>1.25</v>
       </c>
       <c r="L48" s="13">
@@ -11879,37 +11879,37 @@
         <v>0.234375</v>
       </c>
       <c r="O48" s="10">
-        <f>MAX(1,$C48*N48)</f>
-        <v>1</v>
+        <f>$C48*N48</f>
+        <v>0</v>
       </c>
       <c r="P48" s="13">
         <f>$D48*O48</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="36">
         <f t="shared" ref="Q48:Q55" si="32">$E48*P48</f>
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="R48" s="9">
         <v>0.5</v>
       </c>
       <c r="S48" s="10">
-        <f>MAX(1,$C48*R48)</f>
-        <v>1</v>
+        <f>$C48*R48</f>
+        <v>0.625</v>
       </c>
       <c r="T48" s="13">
         <f>$D48*S48</f>
-        <v>0.75</v>
+        <v>0.46875</v>
       </c>
       <c r="U48" s="36">
         <f t="shared" ref="U48:U55" si="33">$E48*T48</f>
-        <v>0.1875</v>
+        <v>0.1171875</v>
       </c>
       <c r="V48" s="9">
         <v>1</v>
       </c>
       <c r="W48" s="10">
-        <f>MAX(1,$C48*V48)</f>
+        <f>$C48*V48</f>
         <v>1.25</v>
       </c>
       <c r="X48" s="13">
@@ -11924,16 +11924,16 @@
         <v>0.5</v>
       </c>
       <c r="AA48" s="10">
-        <f>MAX(1,$C48*Z48)</f>
-        <v>1</v>
+        <f>$C48*Z48</f>
+        <v>0.625</v>
       </c>
       <c r="AB48" s="13">
         <f>$D48*AA48</f>
-        <v>0.75</v>
+        <v>0.46875</v>
       </c>
       <c r="AC48" s="36">
         <f t="shared" ref="AC48:AC55" si="35">$E48*AB48</f>
-        <v>0.1875</v>
+        <v>0.1171875</v>
       </c>
     </row>
     <row r="49" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -11956,11 +11956,11 @@
         <v>70</v>
       </c>
       <c r="G49" s="10">
-        <f>MIN(100,MAX(25,$C49*F49))</f>
+        <f>$C49*F49</f>
         <v>87.5</v>
       </c>
       <c r="H49" s="13">
-        <f t="shared" ref="H49:H55" si="36">$D49*G49</f>
+        <f>$D49*G49</f>
         <v>65.625</v>
       </c>
       <c r="I49" s="36">
@@ -11971,11 +11971,11 @@
         <v>50</v>
       </c>
       <c r="K49" s="10">
-        <f>MIN(100,MAX(25,$C49*J49))</f>
+        <f>$C49*J49</f>
         <v>62.5</v>
       </c>
       <c r="L49" s="13">
-        <f t="shared" ref="L49:L55" si="37">$D49*K49</f>
+        <f>$D49*K49</f>
         <v>46.875</v>
       </c>
       <c r="M49" s="36">
@@ -11983,26 +11983,26 @@
         <v>11.71875</v>
       </c>
       <c r="O49" s="10">
-        <f>MIN(100,MAX(25,$C49*N49))</f>
-        <v>25</v>
+        <f>$C49*N49</f>
+        <v>0</v>
       </c>
       <c r="P49" s="13">
-        <f t="shared" ref="P49:P55" si="38">$D49*O49</f>
-        <v>18.75</v>
+        <f>$D49*O49</f>
+        <v>0</v>
       </c>
       <c r="Q49" s="36">
         <f t="shared" si="32"/>
-        <v>4.6875</v>
+        <v>0</v>
       </c>
       <c r="R49" s="9">
         <v>30</v>
       </c>
       <c r="S49" s="10">
-        <f>MIN(100,MAX(25,$C49*R49))</f>
+        <f>$C49*R49</f>
         <v>37.5</v>
       </c>
       <c r="T49" s="13">
-        <f t="shared" ref="T49:T55" si="39">$D49*S49</f>
+        <f>$D49*S49</f>
         <v>28.125</v>
       </c>
       <c r="U49" s="36">
@@ -12013,11 +12013,11 @@
         <v>40</v>
       </c>
       <c r="W49" s="10">
-        <f>MIN(100,MAX(25,$C49*V49))</f>
+        <f>$C49*V49</f>
         <v>50</v>
       </c>
       <c r="X49" s="13">
-        <f t="shared" ref="X49:X55" si="40">$D49*W49</f>
+        <f>$D49*W49</f>
         <v>37.5</v>
       </c>
       <c r="Y49" s="36">
@@ -12028,16 +12028,16 @@
         <v>15</v>
       </c>
       <c r="AA49" s="10">
-        <f>MIN(100,MAX(25,$C49*Z49))</f>
-        <v>25</v>
+        <f>$C49*Z49</f>
+        <v>18.75</v>
       </c>
       <c r="AB49" s="13">
-        <f t="shared" ref="AB49:AB55" si="41">$D49*AA49</f>
-        <v>18.75</v>
+        <f>$D49*AA49</f>
+        <v>14.0625</v>
       </c>
       <c r="AC49" s="36">
         <f t="shared" si="35"/>
-        <v>4.6875</v>
+        <v>3.515625</v>
       </c>
     </row>
     <row r="50" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -12064,7 +12064,7 @@
         <v>3</v>
       </c>
       <c r="H50" s="13">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="H49:H55" si="36">$D50*G50</f>
         <v>2.25</v>
       </c>
       <c r="I50" s="36">
@@ -12079,7 +12079,7 @@
         <v>1.5</v>
       </c>
       <c r="L50" s="13">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="L50:L56" si="37">$D50*K50</f>
         <v>1.125</v>
       </c>
       <c r="M50" s="36">
@@ -12091,7 +12091,7 @@
         <v>0</v>
       </c>
       <c r="P50" s="13">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="P50:P56" si="38">$D50*O50</f>
         <v>0</v>
       </c>
       <c r="Q50" s="36">
@@ -12106,7 +12106,7 @@
         <v>0.75</v>
       </c>
       <c r="T50" s="13">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="T50:T56" si="39">$D50*S50</f>
         <v>0.5625</v>
       </c>
       <c r="U50" s="36">
@@ -12121,7 +12121,7 @@
         <v>1.5</v>
       </c>
       <c r="X50" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="X50:X56" si="40">$D50*W50</f>
         <v>1.125</v>
       </c>
       <c r="Y50" s="36">
@@ -12136,7 +12136,7 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="AB50" s="13">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="AB50:AB56" si="41">$D50*AA50</f>
         <v>0.33749999999999997</v>
       </c>
       <c r="AC50" s="36">
@@ -12986,7 +12986,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="14">
-        <f t="shared" ref="M59:M79" si="48">L59</f>
+        <f t="shared" ref="M59:M93" si="48">L59</f>
         <v>0</v>
       </c>
       <c r="O59" s="10">
@@ -12998,7 +12998,7 @@
         <v>0</v>
       </c>
       <c r="Q59" s="14">
-        <f t="shared" ref="Q59:Q79" si="49">P59</f>
+        <f t="shared" ref="Q59:Q93" si="49">P59</f>
         <v>0</v>
       </c>
       <c r="R59" s="9">
@@ -13013,7 +13013,7 @@
         <v>3.5</v>
       </c>
       <c r="U59" s="14">
-        <f t="shared" ref="U59:U79" si="50">T59</f>
+        <f t="shared" ref="U59:U93" si="50">T59</f>
         <v>3.5</v>
       </c>
       <c r="W59" s="10">
@@ -13025,7 +13025,7 @@
         <v>3.5</v>
       </c>
       <c r="Y59" s="14">
-        <f t="shared" ref="Y59:Y79" si="51">X59</f>
+        <f t="shared" ref="Y59:Y93" si="51">X59</f>
         <v>3.5</v>
       </c>
       <c r="AA59" s="10">
@@ -13037,7 +13037,7 @@
         <v>0</v>
       </c>
       <c r="AC59" s="14">
-        <f t="shared" ref="AC59:AC79" si="52">AB59</f>
+        <f t="shared" ref="AC59:AC93" si="52">AB59</f>
         <v>0</v>
       </c>
     </row>
@@ -13160,7 +13160,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="13">
-        <f t="shared" ref="L61:L85" si="53">K61</f>
+        <f t="shared" ref="L61:L93" si="53">K61</f>
         <v>0</v>
       </c>
       <c r="M61" s="14">
@@ -13172,7 +13172,7 @@
         <v>0</v>
       </c>
       <c r="P61" s="13">
-        <f t="shared" ref="P61:P85" si="54">O61</f>
+        <f t="shared" ref="P61:P93" si="54">O61</f>
         <v>0</v>
       </c>
       <c r="Q61" s="14">
@@ -13187,7 +13187,7 @@
         <v>50</v>
       </c>
       <c r="T61" s="13">
-        <f t="shared" ref="T61:T85" si="55">S61</f>
+        <f t="shared" ref="T61:T93" si="55">S61</f>
         <v>50</v>
       </c>
       <c r="U61" s="14">
@@ -13199,7 +13199,7 @@
         <v>0</v>
       </c>
       <c r="X61" s="13">
-        <f t="shared" ref="X61:X85" si="56">W61</f>
+        <f t="shared" ref="X61:X93" si="56">W61</f>
         <v>0</v>
       </c>
       <c r="Y61" s="14">
@@ -13211,7 +13211,7 @@
         <v>0</v>
       </c>
       <c r="AB61" s="13">
-        <f t="shared" ref="AB61:AB85" si="57">AA61</f>
+        <f t="shared" ref="AB61:AB93" si="57">AA61</f>
         <v>0</v>
       </c>
       <c r="AC61" s="14">
@@ -15071,7 +15071,7 @@
         <v>0</v>
       </c>
       <c r="K82" s="10">
-        <f t="shared" ref="K82:K85" si="60">J82</f>
+        <f t="shared" ref="K82:K93" si="60">J82</f>
         <v>0</v>
       </c>
       <c r="L82" s="13">
@@ -15083,7 +15083,7 @@
         <v>0</v>
       </c>
       <c r="O82" s="10">
-        <f t="shared" ref="O82:O85" si="62">N82</f>
+        <f t="shared" ref="O82:O93" si="62">N82</f>
         <v>0</v>
       </c>
       <c r="P82" s="13">
@@ -15098,7 +15098,7 @@
         <v>2.5</v>
       </c>
       <c r="S82" s="10">
-        <f t="shared" ref="S82:S85" si="64">R82</f>
+        <f t="shared" ref="S82:S93" si="64">R82</f>
         <v>2.5</v>
       </c>
       <c r="T82" s="13">
@@ -15113,7 +15113,7 @@
         <v>1</v>
       </c>
       <c r="W82" s="10">
-        <f t="shared" ref="W82:W85" si="66">V82</f>
+        <f t="shared" ref="W82:W93" si="66">V82</f>
         <v>1</v>
       </c>
       <c r="X82" s="13">
@@ -15125,7 +15125,7 @@
         <v>1</v>
       </c>
       <c r="AA82" s="10">
-        <f t="shared" ref="AA82:AA85" si="68">Z82</f>
+        <f t="shared" ref="AA82:AA93" si="68">Z82</f>
         <v>0</v>
       </c>
       <c r="AB82" s="13">
@@ -15420,11 +15420,11 @@
         <v>0.5</v>
       </c>
       <c r="G86" s="10">
-        <f>$C86*F86</f>
-        <v>0</v>
+        <f>F86</f>
+        <v>0.5</v>
       </c>
       <c r="H86" s="13">
-        <f>$D86*F86</f>
+        <f>$D86*G86</f>
         <v>0.625</v>
       </c>
       <c r="I86" s="14">
@@ -15435,11 +15435,11 @@
         <v>0.4</v>
       </c>
       <c r="K86" s="10">
-        <f>$C86*J86</f>
-        <v>0</v>
+        <f>J86</f>
+        <v>0.4</v>
       </c>
       <c r="L86" s="13">
-        <f>$D86*J86</f>
+        <f>$D86*K86</f>
         <v>0.5</v>
       </c>
       <c r="M86" s="14">
@@ -15450,11 +15450,11 @@
         <v>0.2</v>
       </c>
       <c r="O86" s="10">
-        <f>$C86*N86</f>
-        <v>0</v>
+        <f>N86</f>
+        <v>0.2</v>
       </c>
       <c r="P86" s="13">
-        <f>$D86*N86</f>
+        <f>$D86*O86</f>
         <v>0.25</v>
       </c>
       <c r="Q86" s="14">
@@ -15465,11 +15465,11 @@
         <v>4</v>
       </c>
       <c r="S86" s="10">
-        <f>$C86*R86</f>
-        <v>0</v>
+        <f>R86</f>
+        <v>4</v>
       </c>
       <c r="T86" s="13">
-        <f>$D86*R86</f>
+        <f>$D86*S86</f>
         <v>5</v>
       </c>
       <c r="U86" s="14">
@@ -15480,11 +15480,11 @@
         <v>1</v>
       </c>
       <c r="W86" s="10">
-        <f>$C86*V86</f>
-        <v>0</v>
+        <f>V86</f>
+        <v>1</v>
       </c>
       <c r="X86" s="13">
-        <f>$D86*V86</f>
+        <f>$D86*W86</f>
         <v>1.25</v>
       </c>
       <c r="Y86" s="14">
@@ -15495,11 +15495,11 @@
         <v>1.5</v>
       </c>
       <c r="AA86" s="10">
-        <f>$C86*Z86</f>
-        <v>0</v>
+        <f>Z86</f>
+        <v>1.5</v>
       </c>
       <c r="AB86" s="13">
-        <f>$D86*Z86</f>
+        <f>$D86*AA86</f>
         <v>1.875</v>
       </c>
       <c r="AC86" s="14">
@@ -15523,11 +15523,11 @@
         <v>70</v>
       </c>
       <c r="G87" s="10">
-        <f>$C87*F87</f>
-        <v>0</v>
+        <f>F87</f>
+        <v>70</v>
       </c>
       <c r="H87" s="13">
-        <f>MIN(100,$D87*F87)</f>
+        <f>$D87*G87</f>
         <v>87.5</v>
       </c>
       <c r="I87" s="14">
@@ -15538,11 +15538,11 @@
         <v>60</v>
       </c>
       <c r="K87" s="10">
-        <f>$C87*J87</f>
-        <v>0</v>
+        <f>J87</f>
+        <v>60</v>
       </c>
       <c r="L87" s="13">
-        <f>MIN(100,$D87*J87)</f>
+        <f>$D87*K87</f>
         <v>75</v>
       </c>
       <c r="M87" s="14">
@@ -15553,11 +15553,11 @@
         <v>70</v>
       </c>
       <c r="O87" s="10">
-        <f>$C87*N87</f>
-        <v>0</v>
+        <f>N87</f>
+        <v>70</v>
       </c>
       <c r="P87" s="13">
-        <f>MIN(100,$D87*N87)</f>
+        <f>$D87*O87</f>
         <v>87.5</v>
       </c>
       <c r="Q87" s="14">
@@ -15568,41 +15568,41 @@
         <v>100</v>
       </c>
       <c r="S87" s="10">
-        <f>$C87*R87</f>
-        <v>0</v>
+        <f>R87</f>
+        <v>100</v>
       </c>
       <c r="T87" s="13">
-        <f>MIN(100,$D87*R87)</f>
-        <v>100</v>
+        <f>$D87*S87</f>
+        <v>125</v>
       </c>
       <c r="U87" s="14">
         <f t="shared" si="65"/>
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="V87" s="9">
         <v>90</v>
       </c>
       <c r="W87" s="10">
-        <f>$C87*V87</f>
-        <v>0</v>
+        <f>V87</f>
+        <v>90</v>
       </c>
       <c r="X87" s="13">
-        <f>MIN(100,$D87*V87)</f>
-        <v>100</v>
+        <f>$D87*W87</f>
+        <v>112.5</v>
       </c>
       <c r="Y87" s="14">
         <f t="shared" si="67"/>
-        <v>100</v>
+        <v>112.5</v>
       </c>
       <c r="Z87" s="9">
         <v>70</v>
       </c>
       <c r="AA87" s="10">
-        <f>$C87*Z87</f>
-        <v>0</v>
+        <f>Z87</f>
+        <v>70</v>
       </c>
       <c r="AB87" s="13">
-        <f>MIN(100,$D87*Z87)</f>
+        <f>$D87*AA87</f>
         <v>87.5</v>
       </c>
       <c r="AC87" s="14">
@@ -18702,8 +18702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC951"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="T1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19053,7 +19053,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="16">
-        <f t="shared" ref="M4:M34" si="3">L4</f>
+        <f t="shared" ref="M4:M67" si="3">L4</f>
         <v>0</v>
       </c>
       <c r="O4" s="39">
@@ -19065,7 +19065,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="16">
-        <f t="shared" ref="Q4:Q34" si="5">P4</f>
+        <f t="shared" ref="Q4:Q67" si="5">P4</f>
         <v>0</v>
       </c>
       <c r="R4" s="9">
@@ -19080,7 +19080,7 @@
         <v>4</v>
       </c>
       <c r="U4" s="16">
-        <f t="shared" ref="U4:U34" si="7">T4</f>
+        <f t="shared" ref="U4:U67" si="7">T4</f>
         <v>4</v>
       </c>
       <c r="V4" s="9">
@@ -19095,7 +19095,7 @@
         <v>20</v>
       </c>
       <c r="Y4" s="16">
-        <f t="shared" ref="Y4:Y34" si="9">X4</f>
+        <f t="shared" ref="Y4:Y67" si="9">X4</f>
         <v>20</v>
       </c>
       <c r="Z4" s="9">
@@ -19110,7 +19110,7 @@
         <v>55</v>
       </c>
       <c r="AC4" s="16">
-        <f t="shared" ref="AC4:AC34" si="11">AB4</f>
+        <f t="shared" ref="AC4:AC67" si="11">AB4</f>
         <v>55</v>
       </c>
     </row>
@@ -21992,7 +21992,7 @@
         <v>77.349999999999994</v>
       </c>
       <c r="M36" s="16">
-        <f t="shared" ref="M36:M37" si="18">L36</f>
+        <f t="shared" ref="M36:M93" si="18">L36</f>
         <v>77.349999999999994</v>
       </c>
       <c r="N36" s="9">
@@ -22007,7 +22007,7 @@
         <v>91</v>
       </c>
       <c r="Q36" s="16">
-        <f t="shared" ref="Q36:Q37" si="19">P36</f>
+        <f t="shared" ref="Q36:Q93" si="19">P36</f>
         <v>91</v>
       </c>
       <c r="R36" s="9">
@@ -22022,7 +22022,7 @@
         <v>81.899999999999991</v>
       </c>
       <c r="U36" s="16">
-        <f t="shared" ref="U36:U37" si="20">T36</f>
+        <f t="shared" ref="U36:U93" si="20">T36</f>
         <v>81.899999999999991</v>
       </c>
       <c r="V36" s="9">
@@ -22037,7 +22037,7 @@
         <v>77.349999999999994</v>
       </c>
       <c r="Y36" s="16">
-        <f t="shared" ref="Y36:Y37" si="21">X36</f>
+        <f t="shared" ref="Y36:Y93" si="21">X36</f>
         <v>77.349999999999994</v>
       </c>
       <c r="Z36" s="9">
@@ -22052,7 +22052,7 @@
         <v>81.899999999999991</v>
       </c>
       <c r="AC36" s="16">
-        <f t="shared" ref="AC36:AC37" si="22">AB36</f>
+        <f t="shared" ref="AC36:AC93" si="22">AB36</f>
         <v>81.899999999999991</v>
       </c>
     </row>
@@ -22378,7 +22378,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="44">
-        <f t="shared" ref="M40:M47" si="23">L40</f>
+        <f t="shared" ref="M40:M93" si="23">L40</f>
         <v>0</v>
       </c>
       <c r="N40" s="9">
@@ -22393,7 +22393,7 @@
         <v>2</v>
       </c>
       <c r="Q40" s="44">
-        <f t="shared" ref="Q40:Q47" si="24">P40</f>
+        <f t="shared" ref="Q40:Q93" si="24">P40</f>
         <v>2</v>
       </c>
       <c r="R40" s="9">
@@ -22408,7 +22408,7 @@
         <v>1</v>
       </c>
       <c r="U40" s="44">
-        <f t="shared" ref="U40:U47" si="25">T40</f>
+        <f t="shared" ref="U40:U93" si="25">T40</f>
         <v>1</v>
       </c>
       <c r="V40" s="9">
@@ -22423,7 +22423,7 @@
         <v>2.5</v>
       </c>
       <c r="Y40" s="44">
-        <f t="shared" ref="Y40:Y47" si="26">X40</f>
+        <f t="shared" ref="Y40:Y93" si="26">X40</f>
         <v>2.5</v>
       </c>
       <c r="Z40" s="9">
@@ -22438,7 +22438,7 @@
         <v>2</v>
       </c>
       <c r="AC40" s="44">
-        <f t="shared" ref="AC40:AC47" si="27">AB40</f>
+        <f t="shared" ref="AC40:AC93" si="27">AB40</f>
         <v>2</v>
       </c>
     </row>
@@ -23059,7 +23059,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="40">
-        <f t="shared" ref="L47" si="35">K47</f>
+        <f t="shared" ref="L47:L93" si="35">K47</f>
         <v>0</v>
       </c>
       <c r="M47" s="16">
@@ -23074,7 +23074,7 @@
         <v>70</v>
       </c>
       <c r="P47" s="40">
-        <f t="shared" ref="P47" si="36">O47</f>
+        <f t="shared" ref="P47:P93" si="36">O47</f>
         <v>70</v>
       </c>
       <c r="Q47" s="16">
@@ -23089,7 +23089,7 @@
         <v>90</v>
       </c>
       <c r="T47" s="40">
-        <f t="shared" ref="T47" si="37">S47</f>
+        <f t="shared" ref="T47:T93" si="37">S47</f>
         <v>90</v>
       </c>
       <c r="U47" s="16">
@@ -23101,7 +23101,7 @@
         <v>0</v>
       </c>
       <c r="X47" s="40">
-        <f t="shared" ref="X47" si="38">W47</f>
+        <f t="shared" ref="X47:X93" si="38">W47</f>
         <v>0</v>
       </c>
       <c r="Y47" s="16">
@@ -23116,7 +23116,7 @@
         <v>60</v>
       </c>
       <c r="AB47" s="40">
-        <f t="shared" ref="AB47" si="39">AA47</f>
+        <f t="shared" ref="AB47:AB93" si="39">AA47</f>
         <v>60</v>
       </c>
       <c r="AC47" s="16">
@@ -24274,11 +24274,11 @@
         <v>0</v>
       </c>
       <c r="L59" s="28">
-        <f t="shared" ref="L59:L85" si="58">K59</f>
+        <f t="shared" ref="L59:L93" si="58">K59</f>
         <v>0</v>
       </c>
       <c r="M59" s="16">
-        <f t="shared" ref="M59:M79" si="59">L59</f>
+        <f t="shared" ref="M59:M93" si="59">L59</f>
         <v>0</v>
       </c>
       <c r="O59" s="39">
@@ -24286,11 +24286,11 @@
         <v>0</v>
       </c>
       <c r="P59" s="28">
-        <f t="shared" ref="P59:P85" si="60">O59</f>
+        <f t="shared" ref="P59:P93" si="60">O59</f>
         <v>0</v>
       </c>
       <c r="Q59" s="16">
-        <f t="shared" ref="Q59:Q79" si="61">P59</f>
+        <f t="shared" ref="Q59:Q93" si="61">P59</f>
         <v>0</v>
       </c>
       <c r="R59" s="9">
@@ -24301,11 +24301,11 @@
         <v>3.5</v>
       </c>
       <c r="T59" s="28">
-        <f t="shared" ref="T59:T85" si="62">S59</f>
+        <f t="shared" ref="T59:T93" si="62">S59</f>
         <v>3.5</v>
       </c>
       <c r="U59" s="16">
-        <f t="shared" ref="U59:U79" si="63">T59</f>
+        <f t="shared" ref="U59:U93" si="63">T59</f>
         <v>3.5</v>
       </c>
       <c r="W59" s="39">
@@ -24313,11 +24313,11 @@
         <v>0</v>
       </c>
       <c r="X59" s="28">
-        <f t="shared" ref="X59:X85" si="64">W59</f>
+        <f t="shared" ref="X59:X93" si="64">W59</f>
         <v>0</v>
       </c>
       <c r="Y59" s="16">
-        <f t="shared" ref="Y59:Y79" si="65">X59</f>
+        <f t="shared" ref="Y59:Y93" si="65">X59</f>
         <v>0</v>
       </c>
       <c r="AA59" s="39">
@@ -24325,11 +24325,11 @@
         <v>0</v>
       </c>
       <c r="AB59" s="28">
-        <f t="shared" ref="AB59:AB85" si="66">AA59</f>
+        <f t="shared" ref="AB59:AB93" si="66">AA59</f>
         <v>0</v>
       </c>
       <c r="AC59" s="16">
-        <f t="shared" ref="AC59:AC79" si="67">AB59</f>
+        <f t="shared" ref="AC59:AC93" si="67">AB59</f>
         <v>0</v>
       </c>
     </row>
@@ -29991,8 +29991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30322,72 +30322,72 @@
         <v>20</v>
       </c>
       <c r="K4" s="27">
-        <f t="shared" ref="K4:K5" si="3">J4</f>
+        <f t="shared" ref="K4:K67" si="3">J4</f>
         <v>0</v>
       </c>
       <c r="L4" s="28">
-        <f t="shared" ref="L4:L34" si="4">K4</f>
+        <f t="shared" ref="L4:L67" si="4">K4</f>
         <v>0</v>
       </c>
       <c r="M4" s="14">
-        <f t="shared" ref="M4:M34" si="5">L4</f>
+        <f t="shared" ref="M4:M67" si="5">L4</f>
         <v>0</v>
       </c>
       <c r="O4" s="27">
-        <f t="shared" ref="O4:O5" si="6">N4</f>
+        <f t="shared" ref="O4:O67" si="6">N4</f>
         <v>0</v>
       </c>
       <c r="P4" s="28">
-        <f t="shared" ref="P4:P34" si="7">O4</f>
+        <f t="shared" ref="P4:P67" si="7">O4</f>
         <v>0</v>
       </c>
       <c r="Q4" s="14">
-        <f t="shared" ref="Q4:Q34" si="8">P4</f>
+        <f t="shared" ref="Q4:Q67" si="8">P4</f>
         <v>0</v>
       </c>
       <c r="R4" s="26">
         <v>4</v>
       </c>
       <c r="S4" s="27">
-        <f t="shared" ref="S4:S5" si="9">R4</f>
+        <f t="shared" ref="S4:S67" si="9">R4</f>
         <v>4</v>
       </c>
       <c r="T4" s="28">
-        <f t="shared" ref="T4:T34" si="10">S4</f>
+        <f t="shared" ref="T4:T67" si="10">S4</f>
         <v>4</v>
       </c>
       <c r="U4" s="14">
-        <f t="shared" ref="U4:U34" si="11">T4</f>
+        <f t="shared" ref="U4:U67" si="11">T4</f>
         <v>4</v>
       </c>
       <c r="V4" s="26">
         <v>20</v>
       </c>
       <c r="W4" s="27">
-        <f t="shared" ref="W4:W5" si="12">V4</f>
+        <f t="shared" ref="W4:W67" si="12">V4</f>
         <v>20</v>
       </c>
       <c r="X4" s="28">
-        <f t="shared" ref="X4:X34" si="13">W4</f>
+        <f t="shared" ref="X4:X67" si="13">W4</f>
         <v>20</v>
       </c>
       <c r="Y4" s="14">
-        <f t="shared" ref="Y4:Y34" si="14">X4</f>
+        <f t="shared" ref="Y4:Y67" si="14">X4</f>
         <v>20</v>
       </c>
       <c r="Z4" s="26">
         <v>55</v>
       </c>
       <c r="AA4" s="27">
-        <f t="shared" ref="AA4:AA5" si="15">Z4</f>
+        <f t="shared" ref="AA4:AA67" si="15">Z4</f>
         <v>55</v>
       </c>
       <c r="AB4" s="28">
-        <f t="shared" ref="AB4:AB34" si="16">AA4</f>
+        <f t="shared" ref="AB4:AB67" si="16">AA4</f>
         <v>55</v>
       </c>
       <c r="AC4" s="14">
-        <f t="shared" ref="AC4:AC34" si="17">AB4</f>
+        <f t="shared" ref="AC4:AC67" si="17">AB4</f>
         <v>55</v>
       </c>
     </row>
@@ -30703,7 +30703,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="27">
-        <f t="shared" ref="K8:K10" si="18">J8</f>
+        <f t="shared" ref="K8:K71" si="18">J8</f>
         <v>0</v>
       </c>
       <c r="L8" s="28">
@@ -30715,7 +30715,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="27">
-        <f t="shared" ref="O8:O10" si="19">N8</f>
+        <f t="shared" ref="O8:O71" si="19">N8</f>
         <v>0</v>
       </c>
       <c r="P8" s="28">
@@ -30727,7 +30727,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="27">
-        <f t="shared" ref="S8:S10" si="20">R8</f>
+        <f t="shared" ref="S8:S71" si="20">R8</f>
         <v>0</v>
       </c>
       <c r="T8" s="28">
@@ -30742,7 +30742,7 @@
         <v>7.5</v>
       </c>
       <c r="W8" s="27">
-        <f t="shared" ref="W8:W10" si="21">V8</f>
+        <f t="shared" ref="W8:W71" si="21">V8</f>
         <v>7.5</v>
       </c>
       <c r="X8" s="28">
@@ -30754,7 +30754,7 @@
         <v>7.5</v>
       </c>
       <c r="AA8" s="27">
-        <f t="shared" ref="AA8:AA10" si="22">Z8</f>
+        <f t="shared" ref="AA8:AA71" si="22">Z8</f>
         <v>0</v>
       </c>
       <c r="AB8" s="28">
@@ -31137,7 +31137,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="27">
-        <f t="shared" ref="K13:K19" si="23">J13</f>
+        <f t="shared" ref="K13:K76" si="23">J13</f>
         <v>0</v>
       </c>
       <c r="L13" s="28">
@@ -31149,7 +31149,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="27">
-        <f t="shared" ref="O13:O19" si="24">N13</f>
+        <f t="shared" ref="O13:O76" si="24">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="28">
@@ -31164,7 +31164,7 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="27">
-        <f t="shared" ref="S13:S19" si="25">R13</f>
+        <f t="shared" ref="S13:S76" si="25">R13</f>
         <v>0.5</v>
       </c>
       <c r="T13" s="28">
@@ -31179,7 +31179,7 @@
         <v>1.7</v>
       </c>
       <c r="W13" s="27">
-        <f t="shared" ref="W13:W19" si="26">V13</f>
+        <f t="shared" ref="W13:W76" si="26">V13</f>
         <v>1.7</v>
       </c>
       <c r="X13" s="28">
@@ -31194,7 +31194,7 @@
         <v>1</v>
       </c>
       <c r="AA13" s="27">
-        <f t="shared" ref="AA13:AA19" si="27">Z13</f>
+        <f t="shared" ref="AA13:AA76" si="27">Z13</f>
         <v>1</v>
       </c>
       <c r="AB13" s="28">
@@ -31866,7 +31866,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="27">
-        <f t="shared" ref="K21:K23" si="28">J21</f>
+        <f t="shared" ref="K21:K84" si="28">J21</f>
         <v>0</v>
       </c>
       <c r="L21" s="28">
@@ -31878,7 +31878,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="27">
-        <f t="shared" ref="O21:O23" si="29">N21</f>
+        <f t="shared" ref="O21:O84" si="29">N21</f>
         <v>0</v>
       </c>
       <c r="P21" s="28">
@@ -31890,7 +31890,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="27">
-        <f t="shared" ref="S21:S23" si="30">R21</f>
+        <f t="shared" ref="S21:S84" si="30">R21</f>
         <v>0</v>
       </c>
       <c r="T21" s="28">
@@ -31905,7 +31905,7 @@
         <v>33.35</v>
       </c>
       <c r="W21" s="27">
-        <f t="shared" ref="W21:W23" si="31">V21</f>
+        <f t="shared" ref="W21:W84" si="31">V21</f>
         <v>33.35</v>
       </c>
       <c r="X21" s="28">
@@ -31917,7 +31917,7 @@
         <v>33.35</v>
       </c>
       <c r="AA21" s="27">
-        <f t="shared" ref="AA21:AA23" si="32">Z21</f>
+        <f t="shared" ref="AA21:AA84" si="32">Z21</f>
         <v>0</v>
       </c>
       <c r="AB21" s="28">
@@ -32300,7 +32300,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="27">
-        <f t="shared" ref="K26:K27" si="33">J26</f>
+        <f t="shared" ref="K26:K89" si="33">J26</f>
         <v>0</v>
       </c>
       <c r="L26" s="28">
@@ -32312,7 +32312,7 @@
         <v>0</v>
       </c>
       <c r="O26" s="27">
-        <f t="shared" ref="O26:O27" si="34">N26</f>
+        <f t="shared" ref="O26:O89" si="34">N26</f>
         <v>0</v>
       </c>
       <c r="P26" s="28">
@@ -32327,7 +32327,7 @@
         <v>3.5</v>
       </c>
       <c r="S26" s="27">
-        <f t="shared" ref="S26:S27" si="35">R26</f>
+        <f t="shared" ref="S26:S89" si="35">R26</f>
         <v>3.5</v>
       </c>
       <c r="T26" s="28">
@@ -32342,7 +32342,7 @@
         <v>11</v>
       </c>
       <c r="W26" s="27">
-        <f t="shared" ref="W26:W27" si="36">V26</f>
+        <f t="shared" ref="W26:W89" si="36">V26</f>
         <v>11</v>
       </c>
       <c r="X26" s="28">
@@ -32357,7 +32357,7 @@
         <v>12</v>
       </c>
       <c r="AA26" s="27">
-        <f t="shared" ref="AA26:AA27" si="37">Z26</f>
+        <f t="shared" ref="AA26:AA89" si="37">Z26</f>
         <v>12</v>
       </c>
       <c r="AB26" s="28">
@@ -32581,7 +32581,7 @@
         <v>9</v>
       </c>
       <c r="K29" s="27">
-        <f t="shared" ref="K29:K30" si="38">J29</f>
+        <f t="shared" ref="K29:K92" si="38">J29</f>
         <v>0</v>
       </c>
       <c r="L29" s="28">
@@ -32593,7 +32593,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="27">
-        <f t="shared" ref="O29:O30" si="39">N29</f>
+        <f t="shared" ref="O29:O92" si="39">N29</f>
         <v>0</v>
       </c>
       <c r="P29" s="28">
@@ -32608,7 +32608,7 @@
         <v>3.5</v>
       </c>
       <c r="S29" s="27">
-        <f t="shared" ref="S29:S30" si="40">R29</f>
+        <f t="shared" ref="S29:S92" si="40">R29</f>
         <v>3.5</v>
       </c>
       <c r="T29" s="28">
@@ -32623,7 +32623,7 @@
         <v>11</v>
       </c>
       <c r="W29" s="27">
-        <f t="shared" ref="W29:W30" si="41">V29</f>
+        <f t="shared" ref="W29:W92" si="41">V29</f>
         <v>11</v>
       </c>
       <c r="X29" s="28">
@@ -32638,7 +32638,7 @@
         <v>10</v>
       </c>
       <c r="AA29" s="27">
-        <f t="shared" ref="AA29:AA30" si="42">Z29</f>
+        <f t="shared" ref="AA29:AA92" si="42">Z29</f>
         <v>10</v>
       </c>
       <c r="AB29" s="28">
@@ -32865,7 +32865,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="27">
-        <f t="shared" ref="K32:K34" si="43">J32</f>
+        <f t="shared" ref="K32:K93" si="43">J32</f>
         <v>0</v>
       </c>
       <c r="L32" s="28">
@@ -32877,7 +32877,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="27">
-        <f t="shared" ref="O32:O34" si="44">N32</f>
+        <f t="shared" ref="O32:O93" si="44">N32</f>
         <v>0</v>
       </c>
       <c r="P32" s="28">
@@ -32892,7 +32892,7 @@
         <v>4</v>
       </c>
       <c r="S32" s="27">
-        <f t="shared" ref="S32:S34" si="45">R32</f>
+        <f t="shared" ref="S32:S93" si="45">R32</f>
         <v>4</v>
       </c>
       <c r="T32" s="28">
@@ -32907,7 +32907,7 @@
         <v>15</v>
       </c>
       <c r="W32" s="27">
-        <f t="shared" ref="W32:W34" si="46">V32</f>
+        <f t="shared" ref="W32:W93" si="46">V32</f>
         <v>15</v>
       </c>
       <c r="X32" s="28">
@@ -32919,7 +32919,7 @@
         <v>15</v>
       </c>
       <c r="AA32" s="27">
-        <f t="shared" ref="AA32:AA34" si="47">Z32</f>
+        <f t="shared" ref="AA32:AA93" si="47">Z32</f>
         <v>0</v>
       </c>
       <c r="AB32" s="28">
@@ -33269,7 +33269,7 @@
         <v>63.75</v>
       </c>
       <c r="M36" s="14">
-        <f t="shared" ref="M36:M49" si="48">L36</f>
+        <f t="shared" ref="M36:M93" si="48">L36</f>
         <v>63.75</v>
       </c>
       <c r="N36" s="26">
@@ -33284,7 +33284,7 @@
         <v>75</v>
       </c>
       <c r="Q36" s="14">
-        <f t="shared" ref="Q36:Q49" si="49">P36</f>
+        <f t="shared" ref="Q36:Q93" si="49">P36</f>
         <v>75</v>
       </c>
       <c r="R36" s="26">
@@ -33299,7 +33299,7 @@
         <v>67.5</v>
       </c>
       <c r="U36" s="14">
-        <f t="shared" ref="U36:U49" si="50">T36</f>
+        <f t="shared" ref="U36:U93" si="50">T36</f>
         <v>67.5</v>
       </c>
       <c r="V36" s="26">
@@ -33314,7 +33314,7 @@
         <v>63.75</v>
       </c>
       <c r="Y36" s="14">
-        <f t="shared" ref="Y36:Y49" si="51">X36</f>
+        <f t="shared" ref="Y36:Y93" si="51">X36</f>
         <v>63.75</v>
       </c>
       <c r="Z36" s="26">
@@ -33329,7 +33329,7 @@
         <v>67.5</v>
       </c>
       <c r="AC36" s="14">
-        <f t="shared" ref="AC36:AC49" si="52">AB36</f>
+        <f t="shared" ref="AC36:AC93" si="52">AB36</f>
         <v>67.5</v>
       </c>
     </row>
@@ -33362,11 +33362,11 @@
         <v>2</v>
       </c>
       <c r="K37" s="27">
-        <f t="shared" ref="K37" si="53">J37</f>
+        <f t="shared" ref="K37:K93" si="53">J37</f>
         <v>2</v>
       </c>
       <c r="L37" s="28">
-        <f t="shared" ref="L37" si="54">K37</f>
+        <f t="shared" ref="L37:L93" si="54">K37</f>
         <v>2</v>
       </c>
       <c r="M37" s="14">
@@ -33374,11 +33374,11 @@
         <v>2</v>
       </c>
       <c r="O37" s="27">
-        <f t="shared" ref="O37" si="55">N37</f>
+        <f t="shared" ref="O37:O93" si="55">N37</f>
         <v>0</v>
       </c>
       <c r="P37" s="28">
-        <f t="shared" ref="P37" si="56">O37</f>
+        <f t="shared" ref="P37:P93" si="56">O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="14">
@@ -33389,11 +33389,11 @@
         <v>1</v>
       </c>
       <c r="S37" s="27">
-        <f t="shared" ref="S37" si="57">R37</f>
+        <f t="shared" ref="S37:S93" si="57">R37</f>
         <v>1</v>
       </c>
       <c r="T37" s="28">
-        <f t="shared" ref="T37" si="58">S37</f>
+        <f t="shared" ref="T37:T93" si="58">S37</f>
         <v>1</v>
       </c>
       <c r="U37" s="14">
@@ -33401,11 +33401,11 @@
         <v>1</v>
       </c>
       <c r="W37" s="27">
-        <f t="shared" ref="W37" si="59">V37</f>
+        <f t="shared" ref="W37:W93" si="59">V37</f>
         <v>0</v>
       </c>
       <c r="X37" s="28">
-        <f t="shared" ref="X37" si="60">W37</f>
+        <f t="shared" ref="X37:X93" si="60">W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="14">
@@ -33413,11 +33413,11 @@
         <v>0</v>
       </c>
       <c r="AA37" s="27">
-        <f t="shared" ref="AA37" si="61">Z37</f>
+        <f t="shared" ref="AA37:AA93" si="61">Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="28">
-        <f t="shared" ref="AB37" si="62">AA37</f>
+        <f t="shared" ref="AB37:AB93" si="62">AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="14">
@@ -33643,11 +33643,11 @@
         <v>0.9</v>
       </c>
       <c r="K40" s="27">
-        <f t="shared" ref="K40:K47" si="63">J40</f>
+        <f t="shared" ref="K40:K93" si="63">J40</f>
         <v>0</v>
       </c>
       <c r="L40" s="28">
-        <f t="shared" ref="L40" si="64">K40</f>
+        <f t="shared" ref="L40:L93" si="64">K40</f>
         <v>0</v>
       </c>
       <c r="M40" s="14">
@@ -33658,11 +33658,11 @@
         <v>2</v>
       </c>
       <c r="O40" s="27">
-        <f t="shared" ref="O40:O47" si="65">N40</f>
+        <f t="shared" ref="O40:O93" si="65">N40</f>
         <v>2</v>
       </c>
       <c r="P40" s="28">
-        <f t="shared" ref="P40" si="66">O40</f>
+        <f t="shared" ref="P40:P93" si="66">O40</f>
         <v>2</v>
       </c>
       <c r="Q40" s="14">
@@ -33673,11 +33673,11 @@
         <v>1</v>
       </c>
       <c r="S40" s="27">
-        <f t="shared" ref="S40:S47" si="67">R40</f>
+        <f t="shared" ref="S40:S93" si="67">R40</f>
         <v>1</v>
       </c>
       <c r="T40" s="28">
-        <f t="shared" ref="T40" si="68">S40</f>
+        <f t="shared" ref="T40:T93" si="68">S40</f>
         <v>1</v>
       </c>
       <c r="U40" s="14">
@@ -33688,11 +33688,11 @@
         <v>2.5</v>
       </c>
       <c r="W40" s="27">
-        <f t="shared" ref="W40:W47" si="69">V40</f>
+        <f t="shared" ref="W40:W93" si="69">V40</f>
         <v>2.5</v>
       </c>
       <c r="X40" s="28">
-        <f t="shared" ref="X40" si="70">W40</f>
+        <f t="shared" ref="X40:X93" si="70">W40</f>
         <v>2.5</v>
       </c>
       <c r="Y40" s="14">
@@ -33703,11 +33703,11 @@
         <v>2</v>
       </c>
       <c r="AA40" s="27">
-        <f t="shared" ref="AA40:AA47" si="71">Z40</f>
+        <f t="shared" ref="AA40:AA93" si="71">Z40</f>
         <v>2</v>
       </c>
       <c r="AB40" s="28">
-        <f t="shared" ref="AB40" si="72">AA40</f>
+        <f t="shared" ref="AB40:AB93" si="72">AA40</f>
         <v>2</v>
       </c>
       <c r="AC40" s="14">
@@ -33945,7 +33945,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="28">
-        <f t="shared" ref="L43:L44" si="73">K43</f>
+        <f t="shared" ref="L43:L93" si="73">K43</f>
         <v>0</v>
       </c>
       <c r="M43" s="14">
@@ -33960,7 +33960,7 @@
         <v>85</v>
       </c>
       <c r="P43" s="28">
-        <f t="shared" ref="P43:P44" si="74">O43</f>
+        <f t="shared" ref="P43:P93" si="74">O43</f>
         <v>85</v>
       </c>
       <c r="Q43" s="14">
@@ -33975,7 +33975,7 @@
         <v>90</v>
       </c>
       <c r="T43" s="28">
-        <f t="shared" ref="T43:T44" si="75">S43</f>
+        <f t="shared" ref="T43:T93" si="75">S43</f>
         <v>90</v>
       </c>
       <c r="U43" s="14">
@@ -33990,7 +33990,7 @@
         <v>80</v>
       </c>
       <c r="X43" s="28">
-        <f t="shared" ref="X43:X44" si="76">W43</f>
+        <f t="shared" ref="X43:X93" si="76">W43</f>
         <v>80</v>
       </c>
       <c r="Y43" s="14">
@@ -34005,7 +34005,7 @@
         <v>60</v>
       </c>
       <c r="AB43" s="28">
-        <f t="shared" ref="AB43:AB44" si="77">AA43</f>
+        <f t="shared" ref="AB43:AB93" si="77">AA43</f>
         <v>60</v>
       </c>
       <c r="AC43" s="14">
@@ -34332,7 +34332,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="28">
-        <f t="shared" ref="L47:L49" si="78">K47</f>
+        <f t="shared" ref="L47:L93" si="78">K47</f>
         <v>0</v>
       </c>
       <c r="M47" s="14">
@@ -34347,7 +34347,7 @@
         <v>70</v>
       </c>
       <c r="P47" s="28">
-        <f t="shared" ref="P47:P49" si="79">O47</f>
+        <f t="shared" ref="P47:P93" si="79">O47</f>
         <v>70</v>
       </c>
       <c r="Q47" s="14">
@@ -34362,7 +34362,7 @@
         <v>90</v>
       </c>
       <c r="T47" s="28">
-        <f t="shared" ref="T47:T49" si="80">S47</f>
+        <f t="shared" ref="T47:T93" si="80">S47</f>
         <v>90</v>
       </c>
       <c r="U47" s="14">
@@ -34374,7 +34374,7 @@
         <v>0</v>
       </c>
       <c r="X47" s="28">
-        <f t="shared" ref="X47:X49" si="81">W47</f>
+        <f t="shared" ref="X47:X93" si="81">W47</f>
         <v>0</v>
       </c>
       <c r="Y47" s="14">
@@ -34389,7 +34389,7 @@
         <v>60</v>
       </c>
       <c r="AB47" s="28">
-        <f t="shared" ref="AB47:AB49" si="82">AA47</f>
+        <f t="shared" ref="AB47:AB93" si="82">AA47</f>
         <v>60</v>
       </c>
       <c r="AC47" s="14">
@@ -35251,7 +35251,7 @@
         <v>20</v>
       </c>
       <c r="K56" s="27">
-        <f t="shared" ref="K56:K79" si="95">J56</f>
+        <f t="shared" ref="K56:K93" si="95">J56</f>
         <v>0</v>
       </c>
       <c r="L56" s="13">
@@ -35263,7 +35263,7 @@
         <v>1.875</v>
       </c>
       <c r="O56" s="27">
-        <f t="shared" ref="O56:O79" si="96">N56</f>
+        <f t="shared" ref="O56:O93" si="96">N56</f>
         <v>0</v>
       </c>
       <c r="P56" s="13">
@@ -35278,7 +35278,7 @@
         <v>0.5</v>
       </c>
       <c r="S56" s="27">
-        <f t="shared" ref="S56:S79" si="97">R56</f>
+        <f t="shared" ref="S56:S93" si="97">R56</f>
         <v>0.5</v>
       </c>
       <c r="T56" s="13">
@@ -35293,7 +35293,7 @@
         <v>0.75</v>
       </c>
       <c r="W56" s="27">
-        <f t="shared" ref="W56:W79" si="98">V56</f>
+        <f t="shared" ref="W56:W93" si="98">V56</f>
         <v>0.75</v>
       </c>
       <c r="X56" s="13">
@@ -35305,7 +35305,7 @@
         <v>1.5</v>
       </c>
       <c r="AA56" s="27">
-        <f t="shared" ref="AA56:AA79" si="99">Z56</f>
+        <f t="shared" ref="AA56:AA93" si="99">Z56</f>
         <v>0</v>
       </c>
       <c r="AB56" s="13">
@@ -35539,11 +35539,11 @@
         <v>0</v>
       </c>
       <c r="L59" s="28">
-        <f t="shared" ref="L59:L85" si="100">K59</f>
+        <f t="shared" ref="L59:L93" si="100">K59</f>
         <v>0</v>
       </c>
       <c r="M59" s="14">
-        <f t="shared" ref="M59:M79" si="101">L59</f>
+        <f t="shared" ref="M59:M93" si="101">L59</f>
         <v>0</v>
       </c>
       <c r="O59" s="27">
@@ -35551,11 +35551,11 @@
         <v>0</v>
       </c>
       <c r="P59" s="28">
-        <f t="shared" ref="P59:P85" si="102">O59</f>
+        <f t="shared" ref="P59:P93" si="102">O59</f>
         <v>0</v>
       </c>
       <c r="Q59" s="14">
-        <f t="shared" ref="Q59:Q79" si="103">P59</f>
+        <f t="shared" ref="Q59:Q93" si="103">P59</f>
         <v>0</v>
       </c>
       <c r="R59" s="26">
@@ -35566,11 +35566,11 @@
         <v>3.5</v>
       </c>
       <c r="T59" s="28">
-        <f t="shared" ref="T59:T85" si="104">S59</f>
+        <f t="shared" ref="T59:T93" si="104">S59</f>
         <v>3.5</v>
       </c>
       <c r="U59" s="14">
-        <f t="shared" ref="U59:U79" si="105">T59</f>
+        <f t="shared" ref="U59:U93" si="105">T59</f>
         <v>3.5</v>
       </c>
       <c r="W59" s="27">
@@ -35578,11 +35578,11 @@
         <v>0</v>
       </c>
       <c r="X59" s="28">
-        <f t="shared" ref="X59:X85" si="106">W59</f>
+        <f t="shared" ref="X59:X93" si="106">W59</f>
         <v>0</v>
       </c>
       <c r="Y59" s="14">
-        <f t="shared" ref="Y59:Y79" si="107">X59</f>
+        <f t="shared" ref="Y59:Y93" si="107">X59</f>
         <v>0</v>
       </c>
       <c r="AA59" s="27">
@@ -35590,11 +35590,11 @@
         <v>0</v>
       </c>
       <c r="AB59" s="28">
-        <f t="shared" ref="AB59:AB85" si="108">AA59</f>
+        <f t="shared" ref="AB59:AB93" si="108">AA59</f>
         <v>0</v>
       </c>
       <c r="AC59" s="14">
-        <f t="shared" ref="AC59:AC79" si="109">AB59</f>
+        <f t="shared" ref="AC59:AC93" si="109">AB59</f>
         <v>0</v>
       </c>
     </row>
@@ -50295,15 +50295,15 @@
       </c>
       <c r="W48">
         <f>'41_Wind_LowSeverity'!O48</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X48">
         <f>'41_Wind_LowSeverity'!P48</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Y48">
         <f>'41_Wind_LowSeverity'!Q48</f>
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="Z48">
         <f>'42_Wind_ModSeverity'!O48</f>
@@ -50335,15 +50335,15 @@
       </c>
       <c r="AG48">
         <f>'41_Wind_LowSeverity'!S48</f>
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="AH48">
         <f>'41_Wind_LowSeverity'!T48</f>
-        <v>0.75</v>
+        <v>0.46875</v>
       </c>
       <c r="AI48">
         <f>'41_Wind_LowSeverity'!U48</f>
-        <v>0.1875</v>
+        <v>0.1171875</v>
       </c>
       <c r="AJ48">
         <f>'42_Wind_ModSeverity'!S48</f>
@@ -50415,15 +50415,15 @@
       </c>
       <c r="BA48">
         <f>'41_Wind_LowSeverity'!AA48</f>
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="BB48">
         <f>'41_Wind_LowSeverity'!AB48</f>
-        <v>0.75</v>
+        <v>0.46875</v>
       </c>
       <c r="BC48">
         <f>'41_Wind_LowSeverity'!AC48</f>
-        <v>0.1875</v>
+        <v>0.1171875</v>
       </c>
       <c r="BD48">
         <f>'42_Wind_ModSeverity'!AA48</f>
@@ -50541,15 +50541,15 @@
       </c>
       <c r="W49">
         <f>'41_Wind_LowSeverity'!O49</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="X49">
         <f>'41_Wind_LowSeverity'!P49</f>
-        <v>18.75</v>
+        <v>0</v>
       </c>
       <c r="Y49">
         <f>'41_Wind_LowSeverity'!Q49</f>
-        <v>4.6875</v>
+        <v>0</v>
       </c>
       <c r="Z49">
         <f>'42_Wind_ModSeverity'!O49</f>
@@ -50661,15 +50661,15 @@
       </c>
       <c r="BA49">
         <f>'41_Wind_LowSeverity'!AA49</f>
-        <v>25</v>
+        <v>18.75</v>
       </c>
       <c r="BB49">
         <f>'41_Wind_LowSeverity'!AB49</f>
-        <v>18.75</v>
+        <v>14.0625</v>
       </c>
       <c r="BC49">
         <f>'41_Wind_LowSeverity'!AC49</f>
-        <v>4.6875</v>
+        <v>3.515625</v>
       </c>
       <c r="BD49">
         <f>'42_Wind_ModSeverity'!AA49</f>
@@ -59563,7 +59563,7 @@
       </c>
       <c r="C86">
         <f>'41_Wind_LowSeverity'!G86</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D86">
         <f>'41_Wind_LowSeverity'!H86</f>
@@ -59603,7 +59603,7 @@
       </c>
       <c r="M86">
         <f>'41_Wind_LowSeverity'!K86</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N86">
         <f>'41_Wind_LowSeverity'!L86</f>
@@ -59643,7 +59643,7 @@
       </c>
       <c r="W86">
         <f>'41_Wind_LowSeverity'!O86</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="X86">
         <f>'41_Wind_LowSeverity'!P86</f>
@@ -59683,7 +59683,7 @@
       </c>
       <c r="AG86">
         <f>'41_Wind_LowSeverity'!S86</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH86">
         <f>'41_Wind_LowSeverity'!T86</f>
@@ -59723,7 +59723,7 @@
       </c>
       <c r="AQ86">
         <f>'41_Wind_LowSeverity'!W86</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR86">
         <f>'41_Wind_LowSeverity'!X86</f>
@@ -59763,7 +59763,7 @@
       </c>
       <c r="BA86">
         <f>'41_Wind_LowSeverity'!AA86</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BB86">
         <f>'41_Wind_LowSeverity'!AB86</f>
@@ -59809,7 +59809,7 @@
       </c>
       <c r="C87">
         <f>'41_Wind_LowSeverity'!G87</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D87">
         <f>'41_Wind_LowSeverity'!H87</f>
@@ -59849,7 +59849,7 @@
       </c>
       <c r="M87">
         <f>'41_Wind_LowSeverity'!K87</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N87">
         <f>'41_Wind_LowSeverity'!L87</f>
@@ -59889,7 +59889,7 @@
       </c>
       <c r="W87">
         <f>'41_Wind_LowSeverity'!O87</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="X87">
         <f>'41_Wind_LowSeverity'!P87</f>
@@ -59929,15 +59929,15 @@
       </c>
       <c r="AG87">
         <f>'41_Wind_LowSeverity'!S87</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AH87">
         <f>'41_Wind_LowSeverity'!T87</f>
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="AI87">
         <f>'41_Wind_LowSeverity'!U87</f>
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="AJ87">
         <f>'42_Wind_ModSeverity'!S87</f>
@@ -59969,15 +59969,15 @@
       </c>
       <c r="AQ87">
         <f>'41_Wind_LowSeverity'!W87</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AR87">
         <f>'41_Wind_LowSeverity'!X87</f>
-        <v>100</v>
+        <v>112.5</v>
       </c>
       <c r="AS87">
         <f>'41_Wind_LowSeverity'!Y87</f>
-        <v>100</v>
+        <v>112.5</v>
       </c>
       <c r="AT87">
         <f>'42_Wind_ModSeverity'!W87</f>
@@ -60009,7 +60009,7 @@
       </c>
       <c r="BA87">
         <f>'41_Wind_LowSeverity'!AA87</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="BB87">
         <f>'41_Wind_LowSeverity'!AB87</f>

</xml_diff>

<commit_message>
Updated MechAdd specifications and MechRemove, Wind expected values
</commit_message>
<xml_diff>
--- a/specifications/4_Wind/ScriptRules_Wind.xlsx
+++ b/specifications/4_Wind/ScriptRules_Wind.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12465" windowHeight="9930" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12465" windowHeight="9930" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -7428,8 +7428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC951"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="450" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18708,7 +18709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="R1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
@@ -24256,7 +24257,7 @@
         <v>9.6</v>
       </c>
       <c r="G59" s="39">
-        <f t="shared" ref="G57:G79" si="52">F59</f>
+        <f t="shared" ref="G59:G79" si="52">F59</f>
         <v>9.6</v>
       </c>
       <c r="H59" s="28">
@@ -24268,7 +24269,7 @@
         <v>9.6</v>
       </c>
       <c r="K59" s="39">
-        <f t="shared" ref="K59:K81" si="53">J59</f>
+        <f t="shared" ref="K59:K79" si="53">J59</f>
         <v>0</v>
       </c>
       <c r="L59" s="28">
@@ -24280,7 +24281,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="39">
-        <f t="shared" ref="O59:O81" si="56">N59</f>
+        <f t="shared" ref="O59:O79" si="56">N59</f>
         <v>0</v>
       </c>
       <c r="P59" s="28">
@@ -24295,7 +24296,7 @@
         <v>3.5</v>
       </c>
       <c r="S59" s="39">
-        <f t="shared" ref="S59:S81" si="59">R59</f>
+        <f t="shared" ref="S59:S79" si="59">R59</f>
         <v>3.5</v>
       </c>
       <c r="T59" s="28">
@@ -24307,7 +24308,7 @@
         <v>3.5</v>
       </c>
       <c r="W59" s="39">
-        <f t="shared" ref="W59:W81" si="62">V59</f>
+        <f t="shared" ref="W59:W79" si="62">V59</f>
         <v>0</v>
       </c>
       <c r="X59" s="28">
@@ -24319,7 +24320,7 @@
         <v>0</v>
       </c>
       <c r="AA59" s="39">
-        <f t="shared" ref="AA59:AA81" si="65">Z59</f>
+        <f t="shared" ref="AA59:AA79" si="65">Z59</f>
         <v>0</v>
       </c>
       <c r="AB59" s="28">
@@ -29989,10 +29990,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF951"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="450" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomLeft" activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected error in wind low severity specs
</commit_message>
<xml_diff>
--- a/specifications/4_Wind/ScriptRules_Wind.xlsx
+++ b/specifications/4_Wind/ScriptRules_Wind.xlsx
@@ -7431,7 +7431,7 @@
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="450" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="AG2" sqref="AG2"/>
+      <selection pane="bottomLeft" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12380,22 +12380,22 @@
         <v>6</v>
       </c>
       <c r="G53" s="10">
-        <f>IF(OR(F3&gt;3,F8&gt;3),F53,$C53*F53)</f>
-        <v>6</v>
+        <f>IF(OR(F3&gt;3,F8&gt;3),$C53*F53,F53)</f>
+        <v>12</v>
       </c>
       <c r="H53" s="13">
         <f t="shared" si="35"/>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="I53" s="36">
         <f t="shared" si="36"/>
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
       <c r="J53" s="9">
         <v>0</v>
       </c>
       <c r="K53" s="10">
-        <f>IF(OR(J3&gt;3,J8&gt;3),J53,$C53*J53)</f>
+        <f>IF(OR(J3&gt;3,J8&gt;3),$C53*J53,J53)</f>
         <v>0</v>
       </c>
       <c r="L53" s="13">
@@ -12407,7 +12407,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="10">
-        <f>IF(OR(N3&gt;3,N8&gt;3),N53,$C53*N53)</f>
+        <f>IF(OR(N3&gt;3,N8&gt;3),$C53*N53,N53)</f>
         <v>0</v>
       </c>
       <c r="P53" s="13">
@@ -12422,46 +12422,46 @@
         <v>1</v>
       </c>
       <c r="S53" s="10">
-        <f>IF(OR(R3&gt;3,R8&gt;3),R53,$C53*R53)</f>
-        <v>2</v>
+        <f>IF(OR(R3&gt;3,R8&gt;3),$C53*R53,R53)</f>
+        <v>1</v>
       </c>
       <c r="T53" s="13">
         <f t="shared" si="41"/>
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="U53" s="36">
         <f t="shared" si="42"/>
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="V53" s="9">
         <v>1.2</v>
       </c>
       <c r="W53" s="10">
-        <f>IF(OR(V3&gt;3,V8&gt;3),V53,$C53*V53)</f>
-        <v>1.2</v>
+        <f>IF(OR(V3&gt;3,V8&gt;3),$C53*V53,V53)</f>
+        <v>2.4</v>
       </c>
       <c r="X53" s="13">
         <f t="shared" si="43"/>
-        <v>0.89999999999999991</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="Y53" s="36">
         <f t="shared" si="44"/>
-        <v>0.44999999999999996</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="Z53" s="9">
         <v>0.5</v>
       </c>
       <c r="AA53" s="10">
-        <f>IF(OR(Z3&gt;3,Z8&gt;3),Z53,$C53*Z53)</f>
-        <v>0.5</v>
+        <f>IF(OR(Z3&gt;3,Z8&gt;3),$C53*Z53,Z53)</f>
+        <v>1</v>
       </c>
       <c r="AB53" s="13">
         <f t="shared" si="45"/>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="AC53" s="36">
         <f t="shared" si="46"/>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="54" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -12484,22 +12484,22 @@
         <v>12</v>
       </c>
       <c r="G54" s="10">
-        <f>IF(OR(F4&gt;9,F9&gt;9),F54,$C54*F54)</f>
-        <v>12</v>
+        <f>IF(OR(F4&gt;9,F9&gt;9),$C54*F54,F54)</f>
+        <v>24</v>
       </c>
       <c r="H54" s="13">
         <f t="shared" si="35"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I54" s="36">
         <f t="shared" si="36"/>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="J54" s="9">
         <v>0</v>
       </c>
       <c r="K54" s="10">
-        <f>IF(OR(J4&gt;9,J9&gt;9),J54,$C54*J54)</f>
+        <f>IF(OR(J4&gt;9,J9&gt;9),$C54*J54,J54)</f>
         <v>0</v>
       </c>
       <c r="L54" s="13">
@@ -12511,7 +12511,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="10">
-        <f>IF(OR(N4&gt;9,N9&gt;9),N54,$C54*N54)</f>
+        <f>IF(OR(N4&gt;9,N9&gt;9),$C54*N54,N54)</f>
         <v>0</v>
       </c>
       <c r="P54" s="13">
@@ -12526,7 +12526,7 @@
         <v>0</v>
       </c>
       <c r="S54" s="10">
-        <f>IF(OR(R4&gt;9,R9&gt;9),R54,$C54*R54)</f>
+        <f>IF(OR(R4&gt;9,R9&gt;9),$C54*R54,R54)</f>
         <v>0</v>
       </c>
       <c r="T54" s="13">
@@ -12541,22 +12541,22 @@
         <v>0.5</v>
       </c>
       <c r="W54" s="10">
-        <f>IF(OR(V4&gt;9,V9&gt;9),V54,$C54*V54)</f>
-        <v>0.5</v>
+        <f>IF(OR(V4&gt;9,V9&gt;9),$C54*V54,V54)</f>
+        <v>1</v>
       </c>
       <c r="X54" s="13">
         <f t="shared" si="43"/>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="Y54" s="36">
         <f t="shared" si="44"/>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="Z54" s="9">
         <v>0</v>
       </c>
       <c r="AA54" s="10">
-        <f>IF(OR(Z4&gt;9,Z9&gt;9),Z54,$C54*Z54)</f>
+        <f>IF(OR(Z4&gt;9,Z9&gt;9),$C54*Z54,Z54)</f>
         <v>0</v>
       </c>
       <c r="AB54" s="13">
@@ -12588,7 +12588,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="10">
-        <f>IF(OR(F5&gt;20,F10&gt;20),F55,$C55*F55)</f>
+        <f>IF(OR(F5&gt;20,F10&gt;20),$C55*F55, F55)</f>
         <v>0</v>
       </c>
       <c r="H55" s="13">
@@ -12603,7 +12603,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="10">
-        <f>IF(OR(J5&gt;20,J10&gt;20),J55,$C55*J55)</f>
+        <f>IF(OR(J5&gt;20,J10&gt;20),$C55*J55, J55)</f>
         <v>0</v>
       </c>
       <c r="L55" s="13">
@@ -12615,7 +12615,7 @@
         <v>0</v>
       </c>
       <c r="O55" s="10">
-        <f>IF(OR(N5&gt;20,N10&gt;20),N55,$C55*N55)</f>
+        <f>IF(OR(N5&gt;20,N10&gt;20),$C55*N55, N55)</f>
         <v>0</v>
       </c>
       <c r="P55" s="13">
@@ -12630,7 +12630,7 @@
         <v>0</v>
       </c>
       <c r="S55" s="10">
-        <f>IF(OR(R5&gt;20,R10&gt;20),R55,$C55*R55)</f>
+        <f>IF(OR(R5&gt;20,R10&gt;20),$C55*R55, R55)</f>
         <v>0</v>
       </c>
       <c r="T55" s="13">
@@ -12645,22 +12645,22 @@
         <v>0.5</v>
       </c>
       <c r="W55" s="10">
-        <f>IF(OR(V5&gt;20,V10&gt;20),V55,$C55*V55)</f>
-        <v>0.5</v>
+        <f>IF(OR(V5&gt;20,V10&gt;20),$C55*V55, V55)</f>
+        <v>1</v>
       </c>
       <c r="X55" s="13">
         <f t="shared" si="43"/>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="Y55" s="36">
         <f t="shared" si="44"/>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="Z55" s="9">
         <v>0</v>
       </c>
       <c r="AA55" s="10">
-        <f>IF(OR(Z5&gt;20,Z10&gt;20),Z55,$C55*Z55)</f>
+        <f>IF(OR(Z5&gt;20,Z10&gt;20),$C55*Z55, Z55)</f>
         <v>0</v>
       </c>
       <c r="AB55" s="13">
@@ -12695,11 +12695,11 @@
       </c>
       <c r="H56" s="13">
         <f>G56+($D56*G53)</f>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="I56" s="14">
         <f>H56+(H53*$E56)</f>
-        <v>8.75</v>
+        <v>12.5</v>
       </c>
       <c r="K56" s="10">
         <f t="shared" ref="K56:K79" si="48">J56</f>
@@ -12734,11 +12734,11 @@
       </c>
       <c r="T56" s="13">
         <f>S56+($D56*S53)</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="U56" s="14">
         <f>T56+(T53*$E56)</f>
-        <v>1.75</v>
+        <v>1.125</v>
       </c>
       <c r="V56" s="9">
         <v>0.75</v>
@@ -12749,11 +12749,11 @@
       </c>
       <c r="X56" s="13">
         <f>W56+($D56*W53)</f>
-        <v>1.05</v>
+        <v>1.35</v>
       </c>
       <c r="Y56" s="14">
         <f>X56+(X53*$E56)</f>
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="AA56" s="10">
         <f t="shared" ref="AA56:AA79" si="52">Z56</f>
@@ -12761,11 +12761,11 @@
       </c>
       <c r="AB56" s="13">
         <f>AA56+($D56*AA53)</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="AC56" s="14">
         <f>AB56+(AB53*$E56)</f>
-        <v>0.3125</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="57" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -12791,11 +12791,11 @@
       </c>
       <c r="H57" s="13">
         <f>G57+($D57*G54)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I57" s="14">
         <f>H57+(H54*$E57)</f>
-        <v>18.5</v>
+        <v>26</v>
       </c>
       <c r="K57" s="10">
         <f t="shared" si="48"/>
@@ -12845,11 +12845,11 @@
       </c>
       <c r="X57" s="13">
         <f>W57+($D57*W54)</f>
-        <v>0.42499999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y57" s="14">
         <f>X57+(X54*$E57)</f>
-        <v>0.61250000000000004</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="AA57" s="10">
         <f t="shared" si="52"/>
@@ -12941,11 +12941,11 @@
       </c>
       <c r="X58" s="13">
         <f>W58+($D58*W55)</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="Y58" s="14">
         <f>X58+(X55*$E58)</f>
-        <v>0.3125</v>
+        <v>0.625</v>
       </c>
       <c r="AA58" s="10">
         <f t="shared" si="52"/>
@@ -18710,8 +18710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF951"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19084,7 +19084,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="16">
-        <f t="shared" ref="P4:P67" si="3">O4</f>
+        <f t="shared" ref="P4:P34" si="3">O4</f>
         <v>0</v>
       </c>
       <c r="R4" s="39">
@@ -19096,7 +19096,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="16">
-        <f t="shared" ref="T4:T67" si="5">S4</f>
+        <f t="shared" ref="T4:T34" si="5">S4</f>
         <v>0</v>
       </c>
       <c r="U4" s="9">
@@ -19111,7 +19111,7 @@
         <v>4</v>
       </c>
       <c r="X4" s="16">
-        <f t="shared" ref="X4:X67" si="7">W4</f>
+        <f t="shared" ref="X4:X34" si="7">W4</f>
         <v>4</v>
       </c>
       <c r="Y4" s="9">
@@ -19126,7 +19126,7 @@
         <v>20</v>
       </c>
       <c r="AB4" s="16">
-        <f t="shared" ref="AB4:AB67" si="9">AA4</f>
+        <f t="shared" ref="AB4:AB34" si="9">AA4</f>
         <v>20</v>
       </c>
       <c r="AC4" s="9">
@@ -19141,7 +19141,7 @@
         <v>55</v>
       </c>
       <c r="AF4" s="16">
-        <f t="shared" ref="AF4:AF67" si="11">AE4</f>
+        <f t="shared" ref="AF4:AF34" si="11">AE4</f>
         <v>55</v>
       </c>
     </row>
@@ -22147,7 +22147,7 @@
         <v>77.349999999999994</v>
       </c>
       <c r="P36" s="16">
-        <f t="shared" ref="P36:P93" si="18">O36</f>
+        <f t="shared" ref="P36:P37" si="18">O36</f>
         <v>77.349999999999994</v>
       </c>
       <c r="Q36" s="9">
@@ -22162,7 +22162,7 @@
         <v>91</v>
       </c>
       <c r="T36" s="16">
-        <f t="shared" ref="T36:T93" si="19">S36</f>
+        <f t="shared" ref="T36:T37" si="19">S36</f>
         <v>91</v>
       </c>
       <c r="U36" s="9">
@@ -22177,7 +22177,7 @@
         <v>81.899999999999991</v>
       </c>
       <c r="X36" s="16">
-        <f t="shared" ref="X36:X93" si="20">W36</f>
+        <f t="shared" ref="X36:X37" si="20">W36</f>
         <v>81.899999999999991</v>
       </c>
       <c r="Y36" s="9">
@@ -22192,7 +22192,7 @@
         <v>77.349999999999994</v>
       </c>
       <c r="AB36" s="16">
-        <f t="shared" ref="AB36:AB93" si="21">AA36</f>
+        <f t="shared" ref="AB36:AB37" si="21">AA36</f>
         <v>77.349999999999994</v>
       </c>
       <c r="AC36" s="9">
@@ -22207,7 +22207,7 @@
         <v>81.899999999999991</v>
       </c>
       <c r="AF36" s="16">
-        <f t="shared" ref="AF36:AF93" si="22">AE36</f>
+        <f t="shared" ref="AF36:AF37" si="22">AE36</f>
         <v>81.899999999999991</v>
       </c>
     </row>
@@ -22557,7 +22557,7 @@
         <v>0</v>
       </c>
       <c r="P40" s="44">
-        <f t="shared" ref="P40:P93" si="23">O40</f>
+        <f t="shared" ref="P40:P47" si="23">O40</f>
         <v>0</v>
       </c>
       <c r="Q40" s="9">
@@ -22572,7 +22572,7 @@
         <v>2</v>
       </c>
       <c r="T40" s="44">
-        <f t="shared" ref="T40:T93" si="24">S40</f>
+        <f t="shared" ref="T40:T47" si="24">S40</f>
         <v>2</v>
       </c>
       <c r="U40" s="9">
@@ -22587,7 +22587,7 @@
         <v>1</v>
       </c>
       <c r="X40" s="44">
-        <f t="shared" ref="X40:X93" si="25">W40</f>
+        <f t="shared" ref="X40:X47" si="25">W40</f>
         <v>1</v>
       </c>
       <c r="Y40" s="9">
@@ -22602,7 +22602,7 @@
         <v>2.5</v>
       </c>
       <c r="AB40" s="44">
-        <f t="shared" ref="AB40:AB93" si="26">AA40</f>
+        <f t="shared" ref="AB40:AB47" si="26">AA40</f>
         <v>2.5</v>
       </c>
       <c r="AC40" s="9">
@@ -22617,7 +22617,7 @@
         <v>2</v>
       </c>
       <c r="AF40" s="44">
-        <f t="shared" ref="AF40:AF93" si="27">AE40</f>
+        <f t="shared" ref="AF40:AF47" si="27">AE40</f>
         <v>2</v>
       </c>
     </row>
@@ -23267,7 +23267,7 @@
         <v>0</v>
       </c>
       <c r="O47" s="40">
-        <f t="shared" ref="O47:O93" si="35">N47</f>
+        <f t="shared" ref="O47" si="35">N47</f>
         <v>0</v>
       </c>
       <c r="P47" s="16">
@@ -23282,7 +23282,7 @@
         <v>70</v>
       </c>
       <c r="S47" s="40">
-        <f t="shared" ref="S47:S93" si="36">R47</f>
+        <f t="shared" ref="S47" si="36">R47</f>
         <v>70</v>
       </c>
       <c r="T47" s="16">
@@ -23297,7 +23297,7 @@
         <v>90</v>
       </c>
       <c r="W47" s="40">
-        <f t="shared" ref="W47:W93" si="37">V47</f>
+        <f t="shared" ref="W47" si="37">V47</f>
         <v>90</v>
       </c>
       <c r="X47" s="16">
@@ -23309,7 +23309,7 @@
         <v>0</v>
       </c>
       <c r="AA47" s="40">
-        <f t="shared" ref="AA47:AA93" si="38">Z47</f>
+        <f t="shared" ref="AA47" si="38">Z47</f>
         <v>0</v>
       </c>
       <c r="AB47" s="16">
@@ -23324,7 +23324,7 @@
         <v>60</v>
       </c>
       <c r="AE47" s="40">
-        <f t="shared" ref="AE47:AE93" si="39">AD47</f>
+        <f t="shared" ref="AE47" si="39">AD47</f>
         <v>60</v>
       </c>
       <c r="AF47" s="16">
@@ -24562,11 +24562,11 @@
         <v>0</v>
       </c>
       <c r="O59" s="28">
-        <f t="shared" ref="O59:O93" si="54">N59</f>
+        <f t="shared" ref="O59:O85" si="54">N59</f>
         <v>0</v>
       </c>
       <c r="P59" s="16">
-        <f t="shared" ref="P59:P93" si="55">O59</f>
+        <f t="shared" ref="P59:P79" si="55">O59</f>
         <v>0</v>
       </c>
       <c r="R59" s="39">
@@ -24574,11 +24574,11 @@
         <v>0</v>
       </c>
       <c r="S59" s="28">
-        <f t="shared" ref="S59:S93" si="57">R59</f>
+        <f t="shared" ref="S59:S85" si="57">R59</f>
         <v>0</v>
       </c>
       <c r="T59" s="16">
-        <f t="shared" ref="T59:T93" si="58">S59</f>
+        <f t="shared" ref="T59:T79" si="58">S59</f>
         <v>0</v>
       </c>
       <c r="U59" s="9">
@@ -24589,11 +24589,11 @@
         <v>3.5</v>
       </c>
       <c r="W59" s="28">
-        <f t="shared" ref="W59:W93" si="60">V59</f>
+        <f t="shared" ref="W59:W85" si="60">V59</f>
         <v>3.5</v>
       </c>
       <c r="X59" s="16">
-        <f t="shared" ref="X59:X93" si="61">W59</f>
+        <f t="shared" ref="X59:X79" si="61">W59</f>
         <v>3.5</v>
       </c>
       <c r="Z59" s="39">
@@ -24601,11 +24601,11 @@
         <v>0</v>
       </c>
       <c r="AA59" s="28">
-        <f t="shared" ref="AA59:AA93" si="63">Z59</f>
+        <f t="shared" ref="AA59:AA85" si="63">Z59</f>
         <v>0</v>
       </c>
       <c r="AB59" s="16">
-        <f t="shared" ref="AB59:AB93" si="64">AA59</f>
+        <f t="shared" ref="AB59:AB79" si="64">AA59</f>
         <v>0</v>
       </c>
       <c r="AD59" s="39">
@@ -24613,11 +24613,11 @@
         <v>0</v>
       </c>
       <c r="AE59" s="28">
-        <f t="shared" ref="AE59:AE93" si="66">AD59</f>
+        <f t="shared" ref="AE59:AE85" si="66">AD59</f>
         <v>0</v>
       </c>
       <c r="AF59" s="16">
-        <f t="shared" ref="AF59:AF93" si="67">AE59</f>
+        <f t="shared" ref="AF59:AF79" si="67">AE59</f>
         <v>0</v>
       </c>
     </row>
@@ -54424,15 +54424,15 @@
       </c>
       <c r="C53">
         <f>'41_Wind_LowSeverity'!G53</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D53">
         <f>'41_Wind_LowSeverity'!H53</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="E53">
         <f>'41_Wind_LowSeverity'!I53</f>
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
       <c r="F53">
         <f>'42_Wind_ModSeverity'!J53</f>
@@ -54544,15 +54544,15 @@
       </c>
       <c r="AG53">
         <f>'41_Wind_LowSeverity'!S53</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH53">
         <f>'41_Wind_LowSeverity'!T53</f>
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="AI53">
         <f>'41_Wind_LowSeverity'!U53</f>
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="AJ53">
         <f>'42_Wind_ModSeverity'!V53</f>
@@ -54584,15 +54584,15 @@
       </c>
       <c r="AQ53">
         <f>'41_Wind_LowSeverity'!W53</f>
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="AR53">
         <f>'41_Wind_LowSeverity'!X53</f>
-        <v>0.89999999999999991</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="AS53">
         <f>'41_Wind_LowSeverity'!Y53</f>
-        <v>0.44999999999999996</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="AT53">
         <f>'42_Wind_ModSeverity'!Z53</f>
@@ -54624,15 +54624,15 @@
       </c>
       <c r="BA53">
         <f>'41_Wind_LowSeverity'!AA53</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="BB53">
         <f>'41_Wind_LowSeverity'!AB53</f>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="BC53">
         <f>'41_Wind_LowSeverity'!AC53</f>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="BD53">
         <f>'42_Wind_ModSeverity'!AD53</f>
@@ -54670,15 +54670,15 @@
       </c>
       <c r="C54">
         <f>'41_Wind_LowSeverity'!G54</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D54">
         <f>'41_Wind_LowSeverity'!H54</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E54">
         <f>'41_Wind_LowSeverity'!I54</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="F54">
         <f>'42_Wind_ModSeverity'!J54</f>
@@ -54830,15 +54830,15 @@
       </c>
       <c r="AQ54">
         <f>'41_Wind_LowSeverity'!W54</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AR54">
         <f>'41_Wind_LowSeverity'!X54</f>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="AS54">
         <f>'41_Wind_LowSeverity'!Y54</f>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="AT54">
         <f>'42_Wind_ModSeverity'!Z54</f>
@@ -55076,15 +55076,15 @@
       </c>
       <c r="AQ55">
         <f>'41_Wind_LowSeverity'!W55</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AR55">
         <f>'41_Wind_LowSeverity'!X55</f>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="AS55">
         <f>'41_Wind_LowSeverity'!Y55</f>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="AT55">
         <f>'42_Wind_ModSeverity'!Z55</f>
@@ -55166,11 +55166,11 @@
       </c>
       <c r="D56">
         <f>'41_Wind_LowSeverity'!H56</f>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="E56">
         <f>'41_Wind_LowSeverity'!I56</f>
-        <v>8.75</v>
+        <v>12.5</v>
       </c>
       <c r="F56">
         <f>'42_Wind_ModSeverity'!J56</f>
@@ -55286,11 +55286,11 @@
       </c>
       <c r="AH56">
         <f>'41_Wind_LowSeverity'!T56</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AI56">
         <f>'41_Wind_LowSeverity'!U56</f>
-        <v>1.75</v>
+        <v>1.125</v>
       </c>
       <c r="AJ56">
         <f>'42_Wind_ModSeverity'!V56</f>
@@ -55326,11 +55326,11 @@
       </c>
       <c r="AR56">
         <f>'41_Wind_LowSeverity'!X56</f>
-        <v>1.05</v>
+        <v>1.35</v>
       </c>
       <c r="AS56">
         <f>'41_Wind_LowSeverity'!Y56</f>
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="AT56">
         <f>'42_Wind_ModSeverity'!Z56</f>
@@ -55366,11 +55366,11 @@
       </c>
       <c r="BB56">
         <f>'41_Wind_LowSeverity'!AB56</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="BC56">
         <f>'41_Wind_LowSeverity'!AC56</f>
-        <v>0.3125</v>
+        <v>0.625</v>
       </c>
       <c r="BD56">
         <f>'42_Wind_ModSeverity'!AD56</f>
@@ -55412,11 +55412,11 @@
       </c>
       <c r="D57">
         <f>'41_Wind_LowSeverity'!H57</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E57">
         <f>'41_Wind_LowSeverity'!I57</f>
-        <v>18.5</v>
+        <v>26</v>
       </c>
       <c r="F57">
         <f>'42_Wind_ModSeverity'!J57</f>
@@ -55572,11 +55572,11 @@
       </c>
       <c r="AR57">
         <f>'41_Wind_LowSeverity'!X57</f>
-        <v>0.42499999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AS57">
         <f>'41_Wind_LowSeverity'!Y57</f>
-        <v>0.61250000000000004</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="AT57">
         <f>'42_Wind_ModSeverity'!Z57</f>
@@ -55818,11 +55818,11 @@
       </c>
       <c r="AR58">
         <f>'41_Wind_LowSeverity'!X58</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="AS58">
         <f>'41_Wind_LowSeverity'!Y58</f>
-        <v>0.3125</v>
+        <v>0.625</v>
       </c>
       <c r="AT58">
         <f>'42_Wind_ModSeverity'!Z58</f>

</xml_diff>

<commit_message>
Corrected hopefully last errors in wind low severity expected
</commit_message>
<xml_diff>
--- a/specifications/4_Wind/ScriptRules_Wind.xlsx
+++ b/specifications/4_Wind/ScriptRules_Wind.xlsx
@@ -7428,10 +7428,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="450" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="AE2" sqref="AE2"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12484,7 +12484,7 @@
         <v>12</v>
       </c>
       <c r="G54" s="10">
-        <f>IF(OR(F4&gt;9,F9&gt;9),$C54*F54,F54)</f>
+        <f>IF(OR(F3&gt;9,F8&gt;9),$C54*F54,F54)</f>
         <v>24</v>
       </c>
       <c r="H54" s="13">
@@ -12499,7 +12499,7 @@
         <v>0</v>
       </c>
       <c r="K54" s="10">
-        <f>IF(OR(J4&gt;9,J9&gt;9),$C54*J54,J54)</f>
+        <f>IF(OR(J3&gt;9,J8&gt;9),$C54*J54,J54)</f>
         <v>0</v>
       </c>
       <c r="L54" s="13">
@@ -12511,7 +12511,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="10">
-        <f>IF(OR(N4&gt;9,N9&gt;9),$C54*N54,N54)</f>
+        <f>IF(OR(N3&gt;9,N8&gt;9),$C54*N54,N54)</f>
         <v>0</v>
       </c>
       <c r="P54" s="13">
@@ -12526,7 +12526,7 @@
         <v>0</v>
       </c>
       <c r="S54" s="10">
-        <f>IF(OR(R4&gt;9,R9&gt;9),$C54*R54,R54)</f>
+        <f>IF(OR(R3&gt;9,R8&gt;9),$C54*R54,R54)</f>
         <v>0</v>
       </c>
       <c r="T54" s="13">
@@ -12541,7 +12541,7 @@
         <v>0.5</v>
       </c>
       <c r="W54" s="10">
-        <f>IF(OR(V4&gt;9,V9&gt;9),$C54*V54,V54)</f>
+        <f>IF(OR(V3&gt;9,V8&gt;9),$C54*V54,V54)</f>
         <v>1</v>
       </c>
       <c r="X54" s="13">
@@ -12556,7 +12556,7 @@
         <v>0</v>
       </c>
       <c r="AA54" s="10">
-        <f>IF(OR(Z4&gt;9,Z9&gt;9),$C54*Z54,Z54)</f>
+        <f>IF(OR(Z3&gt;9,Z8&gt;9),$C54*Z54,Z54)</f>
         <v>0</v>
       </c>
       <c r="AB54" s="13">
@@ -12588,7 +12588,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="10">
-        <f>IF(OR(F5&gt;20,F10&gt;20),$C55*F55, F55)</f>
+        <f>IF(OR(F3&gt;20,F8&gt;20),$C55*F55,F55)</f>
         <v>0</v>
       </c>
       <c r="H55" s="13">
@@ -12603,7 +12603,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="10">
-        <f>IF(OR(J5&gt;20,J10&gt;20),$C55*J55, J55)</f>
+        <f>IF(OR(J3&gt;20,J8&gt;20),$C55*J55,J55)</f>
         <v>0</v>
       </c>
       <c r="L55" s="13">
@@ -12615,7 +12615,7 @@
         <v>0</v>
       </c>
       <c r="O55" s="10">
-        <f>IF(OR(N5&gt;20,N10&gt;20),$C55*N55, N55)</f>
+        <f>IF(OR(N3&gt;20,N8&gt;20),$C55*N55,N55)</f>
         <v>0</v>
       </c>
       <c r="P55" s="13">
@@ -12630,7 +12630,7 @@
         <v>0</v>
       </c>
       <c r="S55" s="10">
-        <f>IF(OR(R5&gt;20,R10&gt;20),$C55*R55, R55)</f>
+        <f>IF(OR(R3&gt;20,R8&gt;20),$C55*R55,R55)</f>
         <v>0</v>
       </c>
       <c r="T55" s="13">
@@ -12645,22 +12645,22 @@
         <v>0.5</v>
       </c>
       <c r="W55" s="10">
-        <f>IF(OR(V5&gt;20,V10&gt;20),$C55*V55, V55)</f>
-        <v>1</v>
+        <f>IF(OR(V3&gt;20,V8&gt;20),$C55*V55,V55)</f>
+        <v>0.5</v>
       </c>
       <c r="X55" s="13">
         <f t="shared" si="43"/>
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="Y55" s="36">
         <f t="shared" si="44"/>
-        <v>0.375</v>
+        <v>0.1875</v>
       </c>
       <c r="Z55" s="9">
         <v>0</v>
       </c>
       <c r="AA55" s="10">
-        <f>IF(OR(Z5&gt;20,Z10&gt;20),$C55*Z55, Z55)</f>
+        <f>IF(OR(Z3&gt;20,Z8&gt;20),$C55*Z55,Z55)</f>
         <v>0</v>
       </c>
       <c r="AB55" s="13">
@@ -12941,11 +12941,11 @@
       </c>
       <c r="X58" s="13">
         <f>W58+($D58*W55)</f>
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="Y58" s="14">
         <f>X58+(X55*$E58)</f>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="AA58" s="10">
         <f t="shared" si="52"/>
@@ -55076,15 +55076,15 @@
       </c>
       <c r="AQ55">
         <f>'41_Wind_LowSeverity'!W55</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AR55">
         <f>'41_Wind_LowSeverity'!X55</f>
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="AS55">
         <f>'41_Wind_LowSeverity'!Y55</f>
-        <v>0.375</v>
+        <v>0.1875</v>
       </c>
       <c r="AT55">
         <f>'42_Wind_ModSeverity'!Z55</f>
@@ -55818,11 +55818,11 @@
       </c>
       <c r="AR58">
         <f>'41_Wind_LowSeverity'!X58</f>
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="AS58">
         <f>'41_Wind_LowSeverity'!Y58</f>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="AT58">
         <f>'42_Wind_ModSeverity'!Z58</f>

</xml_diff>